<commit_message>
Added logic for trade up team
</commit_message>
<xml_diff>
--- a/Files/Madden24/IE/Test/Draft_Trades.xlsx
+++ b/Files/Madden24/IE/Test/Draft_Trades.xlsx
@@ -17365,7 +17365,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>TradeTeam</t>
+          <t>TradeWith</t>
         </is>
       </c>
     </row>
@@ -17394,11 +17394,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -17425,11 +17421,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -17456,11 +17448,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -17487,11 +17475,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -17518,11 +17502,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -17546,14 +17526,10 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Broncos</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -17580,11 +17556,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -17611,11 +17583,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -17642,11 +17610,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -17673,11 +17637,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -17704,11 +17664,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -17735,11 +17691,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -17766,11 +17718,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -17797,11 +17745,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -17828,11 +17772,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -17859,11 +17799,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -17887,12 +17823,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Chiefs</t>
         </is>
       </c>
     </row>
@@ -17921,11 +17857,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -17952,11 +17884,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -17983,11 +17911,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -18014,11 +17938,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -18045,11 +17965,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -18076,11 +17992,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -18107,11 +18019,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -18138,11 +18046,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -18169,11 +18073,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -18200,11 +18100,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -18231,11 +18127,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -18262,11 +18154,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -18293,11 +18181,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -18324,11 +18208,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -18355,11 +18235,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -18386,11 +18262,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -18417,11 +18289,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -18448,11 +18316,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -18476,14 +18340,10 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Patriots</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -18510,11 +18370,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -18541,11 +18397,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -18572,11 +18424,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -18603,11 +18451,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -18634,11 +18478,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -18665,11 +18505,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -18696,11 +18532,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -18727,11 +18559,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -18755,12 +18583,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Bears</t>
         </is>
       </c>
     </row>
@@ -18789,11 +18617,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -18820,11 +18644,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -18851,11 +18671,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -18882,11 +18698,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -18913,11 +18725,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -18944,11 +18752,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -18975,11 +18779,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -19006,11 +18806,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -19037,11 +18833,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -19068,11 +18860,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -19096,12 +18884,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Panthers</t>
         </is>
       </c>
     </row>
@@ -19130,11 +18918,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -19161,11 +18945,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -19189,14 +18969,10 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Chiefs</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -19223,11 +18999,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -19254,11 +19026,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -19285,11 +19053,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -19316,11 +19080,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -19347,11 +19107,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -19378,11 +19134,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -19409,11 +19161,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -19440,11 +19188,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -19471,11 +19215,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -19502,11 +19242,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -19533,11 +19269,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -19564,11 +19296,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -19595,11 +19323,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -19626,11 +19350,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -19657,11 +19377,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -19688,11 +19404,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -19719,11 +19431,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -19750,11 +19458,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -19781,11 +19485,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -19812,11 +19512,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -19843,11 +19539,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -19874,11 +19566,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -19905,11 +19593,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -19936,11 +19620,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -19967,11 +19647,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -19998,11 +19674,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -20029,11 +19701,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -20060,11 +19728,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -20091,11 +19755,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -20122,11 +19782,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -20153,11 +19809,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -20184,11 +19836,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -20215,11 +19863,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -20246,11 +19890,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -20277,11 +19917,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -20308,11 +19944,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -20339,11 +19971,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -20370,11 +19998,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -20401,11 +20025,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -20432,11 +20052,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -20460,14 +20076,10 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>Browns</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -20494,11 +20106,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -20525,11 +20133,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -20556,11 +20160,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -20584,12 +20184,12 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Raiders</t>
         </is>
       </c>
     </row>
@@ -20618,11 +20218,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -20649,11 +20245,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -20680,11 +20272,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -20711,11 +20299,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -20742,11 +20326,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -20770,12 +20350,12 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Bears</t>
         </is>
       </c>
     </row>
@@ -20804,11 +20384,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -20835,11 +20411,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -20866,11 +20438,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -20897,11 +20465,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -20928,11 +20492,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -20956,14 +20516,10 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>Colts</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -20990,11 +20546,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -21018,12 +20570,12 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Jets</t>
         </is>
       </c>
     </row>
@@ -21052,11 +20604,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -21083,11 +20631,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -21114,11 +20658,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -21145,11 +20685,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -21176,11 +20712,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -21207,11 +20739,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -21238,11 +20766,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -21269,11 +20793,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -21300,11 +20820,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -21331,11 +20847,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -21362,11 +20874,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -21393,11 +20901,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -21424,11 +20928,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -21455,11 +20955,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -21483,14 +20979,10 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>Packers</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -21517,11 +21009,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -21548,11 +21036,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -21579,11 +21063,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -21610,11 +21090,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -21641,11 +21117,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -21672,11 +21144,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -21703,11 +21171,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -21734,11 +21198,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -21765,11 +21225,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -21796,11 +21252,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -21824,12 +21276,12 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Bears</t>
         </is>
       </c>
     </row>
@@ -21858,11 +21310,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -21889,11 +21337,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -21920,11 +21364,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -21948,14 +21388,10 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>Raiders</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -21982,11 +21418,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -22013,11 +21445,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -22041,12 +21469,12 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Seahawks</t>
         </is>
       </c>
     </row>
@@ -22075,11 +21503,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -22106,11 +21530,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -22137,11 +21557,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -22168,11 +21584,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -22196,14 +21608,10 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>Ravens</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -22230,11 +21638,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -22258,12 +21662,12 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Patriots</t>
         </is>
       </c>
     </row>
@@ -22292,11 +21696,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -22323,11 +21723,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -22354,11 +21750,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -22385,11 +21777,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -22416,11 +21804,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -22444,14 +21828,10 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>Dolphins</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -22478,11 +21858,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -22509,11 +21885,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -22540,11 +21912,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -22571,11 +21939,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -22602,11 +21966,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G170" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -22633,11 +21993,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G171" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -22664,11 +22020,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G172" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -22695,11 +22047,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G173" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -22726,11 +22074,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G174" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -22757,11 +22101,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G175" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -22788,11 +22128,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G176" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -22819,11 +22155,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G177" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -22850,11 +22182,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G178" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -22881,11 +22209,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G179" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -22912,11 +22236,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G180" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -22943,11 +22263,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G181" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -22974,11 +22290,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G182" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -23005,11 +22317,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G183" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -23036,11 +22344,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G184" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -23067,11 +22371,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G185" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -23098,11 +22398,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G186" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -23129,11 +22425,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G187" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -23160,11 +22452,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G188" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -23191,11 +22479,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G189" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -23222,11 +22506,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G190" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -23250,14 +22530,10 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G191" t="inlineStr">
-        <is>
-          <t>Dolphins</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -23284,11 +22560,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G192" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -23315,11 +22587,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G193" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -23346,11 +22614,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G194" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -23377,11 +22641,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G195" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -23408,11 +22668,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G196" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -23439,11 +22695,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G197" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -23470,11 +22722,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G198" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -23501,11 +22749,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G199" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -23532,11 +22776,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G200" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -23563,11 +22803,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G201" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -23594,11 +22830,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G202" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -23625,11 +22857,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G203" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -23656,11 +22884,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G204" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -23687,11 +22911,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G205" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -23718,11 +22938,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G206" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -23746,14 +22962,10 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G207" t="inlineStr">
-        <is>
-          <t>Browns</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -23780,11 +22992,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G208" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -23811,11 +23019,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G209" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -23842,11 +23046,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G210" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -23873,11 +23073,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G211" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -23904,11 +23100,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G212" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -23935,11 +23127,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G213" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -23963,12 +23151,12 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Titans</t>
         </is>
       </c>
     </row>
@@ -23997,11 +23185,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G215" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -24028,11 +23212,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G216" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -24059,11 +23239,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G217" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -24090,11 +23266,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G218" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -24121,11 +23293,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G219" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -24152,11 +23320,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G220" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -24180,14 +23344,10 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G221" t="inlineStr">
-        <is>
-          <t>Giants</t>
-        </is>
-      </c>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -24214,11 +23374,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G222" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -24245,11 +23401,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G223" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -24276,11 +23428,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G224" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -24307,11 +23455,7 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G225" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G225" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>